<commit_message>
Revised effective exchange rate
</commit_message>
<xml_diff>
--- a/Profits.xlsx
+++ b/Profits.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="780" yWindow="940" windowWidth="27640" windowHeight="16060" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16580" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -424,15 +424,16 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:D127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="200" workbookViewId="0">
+      <selection activeCell="D71" sqref="D71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col width="29.1640625" customWidth="1" min="1" max="1"/>
+    <col width="21" customWidth="1" min="1" max="1"/>
+    <col width="18.1640625" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -451,40 +452,45 @@
           <t>Date</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.2003667213262661</v>
+        <v>0.0008356059995265723</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>POLS</t>
+          <t>WETH</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>5/17/2021</t>
+          <t>5/16/2021</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>36.56979430237686</v>
+        <v>0.4070365657446029</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>USDT</t>
+          <t>POLS</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>5/16/2021</t>
+          <t>5/17/2021</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1.170886935648545</v>
+        <v>2.483514110307883</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -499,7 +505,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4.221238559632442e-05</v>
+        <v>8.497255638487784e-05</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -514,7 +520,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>61.80026544693226</v>
+        <v>125.4230923753032</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -529,7 +535,7 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>16.51656543450235</v>
+        <v>33.05169857256715</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -544,11 +550,11 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1.947692858458904</v>
+        <v>0.000319646871314464</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>FEI</t>
+          <t>WBTC</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -558,9 +564,12 @@
       </c>
     </row>
     <row r="9">
+      <c r="A9" t="n">
+        <v>2.869903625850301e-05</v>
+      </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>TRIBE</t>
+          <t>WBTC</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -571,11 +580,11 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.008841599604244132</v>
+        <v>0.1290241975291226</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>FEI</t>
+          <t>TRIBE</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -585,6 +594,9 @@
       </c>
     </row>
     <row r="11">
+      <c r="A11" t="n">
+        <v>0.0139962788132354</v>
+      </c>
       <c r="B11" t="inlineStr">
         <is>
           <t>UNI</t>
@@ -598,187 +610,187 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1.567811070982657</v>
+        <v>0.9413297525765252</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>RAI</t>
+          <t>UNI</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>5/27/2021</t>
+          <t>5/26/2021</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0.4259670879065869</v>
+        <v>3.146489367810659</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>FEI</t>
+          <t>RAI</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>5/28/2021</t>
+          <t>5/27/2021</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0.6063714202744146</v>
+        <v>0.0006350627805973025</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>USDT</t>
+          <t>WETH</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>5/29/2021</t>
+          <t>5/28/2021</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0.4195484723165173</v>
+        <v>1.27999593174209</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>FEI</t>
+          <t>USDT</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>5/30/2021</t>
+          <t>5/29/2021</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0.0003643070988096683</v>
+        <v>0.8443026101314892</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>WETH</t>
+          <t>FEI</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>5/31/2021</t>
+          <t>5/30/2021</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>4.255878692343619e-06</v>
+        <v>0.0007324189480782707</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>WBTC</t>
+          <t>WETH</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>6/1/2021</t>
+          <t>5/31/2021</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1.912219487007309e-05</v>
+        <v>19.18745452488497</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>UNI</t>
+          <t>FEI</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>6/2/2021</t>
+          <t>6/1/2021</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>0.01614737923715803</v>
+        <v>3.828219539741239e-05</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>LINK</t>
+          <t>UNI</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>6/3/2021</t>
+          <t>6/2/2021</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0.006240848554649014</v>
+        <v>0.03240217618168506</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>DAI</t>
+          <t>LINK</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>6/4/2021</t>
+          <t>6/3/2021</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0.0005886375466919048</v>
+        <v>0.01249698637645436</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>WETH</t>
+          <t>DAI</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>6/6/2021</t>
+          <t>6/4/2021</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>0.04715793045444516</v>
+        <v>0.004954942359160511</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>USDC</t>
+          <t>UNI</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>6/7/2021</t>
+          <t>6/5/2021</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>0.001875229508471438</v>
+        <v>0.001188445342719963</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>MATIC</t>
+          <t>WETH</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>6/8/2021</t>
+          <t>6/6/2021</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>0.01467596451905297</v>
+        <v>0.09530555574891109</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -787,148 +799,148 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>6/9/2021</t>
+          <t>6/7/2021</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>2.246505847754219e-06</v>
+        <v>0.00375779588915498</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>WBTC</t>
+          <t>MATIC</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>6/10/2021</t>
+          <t>6/8/2021</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>0.009053470635694616</v>
+        <v>0.03175779735091099</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>USDT</t>
+          <t>USDC</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>6/11/2021</t>
+          <t>6/9/2021</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>0.00285500366167879</v>
+        <v>0.0001953274074113342</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>UNI</t>
+          <t>WETH</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>6/12/2021</t>
+          <t>6/10/2021</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>7.328190562181488</v>
+        <v>0.01819086570473594</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>DAI</t>
+          <t>USDT</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>6/13/2021</t>
+          <t>6/11/2021</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>0.0001257796148737937</v>
+        <v>0.0006549639283477023</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>UNI</t>
+          <t>WETH</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>6/14/2021</t>
+          <t>6/12/2021</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>0.5070784630303837</v>
+        <v>15.03718026512569</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>DAI</t>
+          <t>USDC</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>6/16/2021</t>
+          <t>6/13/2021</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>0.005476080735208527</v>
+        <v>0.0002519466137180966</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>USDT</t>
+          <t>UNI</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>6/17/2021</t>
+          <t>6/14/2021</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>69.9133995404311</v>
+        <v>0.002624297781600449</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>SHIB</t>
+          <t>NEXO</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>6/18/2021</t>
+          <t>6/15/2021</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>0.9848942138292784</v>
+        <v>1.021286700006836</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>USDC</t>
+          <t>DAI</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>6/19/2021</t>
+          <t>6/16/2021</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>0.6607845781416408</v>
+        <v>0.01117778020845428</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
@@ -937,70 +949,73 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>6/20/2021</t>
+          <t>6/17/2021</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>0.0001235144518106062</v>
+        <v>142.791352943065</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>WETH</t>
+          <t>SHIB</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>6/21/2021</t>
+          <t>6/18/2021</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>7.537681320335293e-08</v>
+        <v>1.978413368459911</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>WBTC</t>
+          <t>USDC</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>6/22/2021</t>
+          <t>6/19/2021</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>465.4093504378875</v>
+        <v>1.328663204882027</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>SHIB</t>
+          <t>USDT</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>6/24/2021</t>
+          <t>6/20/2021</t>
         </is>
       </c>
     </row>
     <row r="38">
+      <c r="A38" t="n">
+        <v>0.0002503347345526614</v>
+      </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>USDC</t>
+          <t>WETH</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>6/25/2021</t>
+          <t>6/21/2021</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>0.0003161936262230324</v>
+        <v>0.0001855939337358607</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
@@ -1009,67 +1024,1315 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>6/26/2021</t>
+          <t>6/22/2021</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>0.08490178441505192</v>
+        <v>0.004794849186580803</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>WETH</t>
+          <t>USDT</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>6/27/2021</t>
+          <t>6/23/2021</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>0.05361507229388707</v>
+        <v>976.6874989004446</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>UNI</t>
+          <t>SHIB</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>6/28/2021</t>
+          <t>6/24/2021</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>0.1067080371552791</v>
+        <v>0.01039777284504212</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>USDT</t>
+          <t>UNI</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>6/29/2021</t>
+          <t>6/25/2021</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>0.0002259773255244794</v>
+        <v>0.0006447197666062821</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
+          <t>WETH</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>6/26/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>0.1712564371667673</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>WETH</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>6/27/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>0.003206253536628539</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
           <t>UNI</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>6/28/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>0.1831307066145058</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>USDT</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>6/29/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>0.01445247339846834</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>USDC</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
         <is>
           <t>6/30/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>0.002275848822266613</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>BUSD</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>7/1/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>0.00173780800637531</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>UNI</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>7/2/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>USDT</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>7/3/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>USDC</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>7/4/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>0.5793049749855186</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>DAI</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>7/5/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>USDC</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>7/6/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>0.1615509175578511</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>USDT</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>7/7/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>0.03732488278599355</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>USDT</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>7/8/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>1167.277592279961</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>USDC</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>7/9/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>USDT</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>7/10/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>0.05698764385913374</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>WETH</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>7/11/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>5.10904604976146e-05</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>WETH</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>7/12/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>79.34391312572512</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>USDC</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>7/13/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>29.48467676765369</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>USDC</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>7/14/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>2.053131060355987</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>USDT</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>7/15/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>0.00600712600453927</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>WETH</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>7/16/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>0.2673113377192706</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>DAI</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>7/17/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>1.384458065968887</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>USDT</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>7/18/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>0.08167241449390694</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>USDT</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>7/19/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>0.0009379589671091662</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>UNI</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>7/20/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>0.3474432442228981</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>USDC</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>7/21/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>0.4805039281991004</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>USDC</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>7/22/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>0.8075921733095717</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>WETH</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>7/23/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>0.1203532099071101</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>USDC</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>7/24/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>0.07103491007406681</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>UNI</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>7/25/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>0.06580576348485412</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>UNI</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>7/26/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>0.0003610515666717679</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>WETH</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>7/27/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>0.02138625967083282</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>DAI</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>7/28/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>0.02661319226089454</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>USDT</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>7/29/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>42.07838485380108</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>DAI</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>7/30/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>0.006467222723287591</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>DAI</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>7/31/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>8.51695046789871</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>LTY</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>8/1/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>0.04337049296046214</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>USDC</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>8/2/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>0.0266101375197316</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>USDT</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>8/3/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>0.000177504721039199</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>WETH</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>8/4/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>942.0678571103208</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>USDT</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>8/5/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>0.007422961080351231</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>WBTC</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>8/6/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>4.799078232293336e-05</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>WETH</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>8/7/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>44.06669043508032</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>USDC</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>8/8/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>0.2432036452832991</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>WETH</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>8/9/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>0.4163286857773578</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>WBTC</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>8/10/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>0.0001643456488278775</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>AAVE</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>8/11/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>46.1765552859531</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>DAI</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>8/12/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>0.01047288540308089</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>EURT</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>8/13/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>8.772451810934272e-05</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>WETH</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>8/14/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>0.3082066954421216</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>WETH</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>8/15/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>0.0005313641921644296</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>USDC</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>8/16/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>7873.063885953547</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>DAI</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>8/17/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>0.03320811859146</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>USDC</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>8/18/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>0.01218930091621862</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>USDC</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>8/19/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>125.0963201698028</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>DAI</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>8/20/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>223.5484963546414</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>USDT</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>8/21/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>1688.465342410133</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>USDC</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>8/22/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>1.625112977518008e-05</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>WETH</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>8/23/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>6.736909749926497</v>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>USDC</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>8/24/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>0.0006813324293630935</v>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>UNI</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>8/25/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>0.7237203756046888</v>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>DAI</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>8/26/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>6.186995604939849e-05</v>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>WETH</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>8/27/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>0.002168056858765338</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>WETH</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>8/28/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>0.0009528145354111214</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>WETH</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>8/29/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>12.99462909843876</v>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>DAI</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>8/30/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>18.82909077232466</v>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>USDT</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>8/31/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>0.02315531904275048</v>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>UNI</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>9/1/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>32.76616439577384</v>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>USDC</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>9/2/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>0.6754694282920966</v>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>USDC</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>9/3/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>0.7998804945749196</v>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>USDC</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>9/4/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>0.001123456289828483</v>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>WETH</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>9/5/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>2.02053587682131</v>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>BADGER</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>9/6/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>2.707378286934237</v>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>BOND</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>9/7/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>0.004059563476130002</v>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>WETH</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>9/8/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>0.1526851064957793</v>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>USDC</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>9/9/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>0.0002106782741790394</v>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>COMP</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>9/10/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>0.0001036999141030576</v>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>USDC</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>9/11/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>8.558359258136946</v>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>USDC</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>9/12/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>0.005937014992505929</v>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>AAVE</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>9/13/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>0.007720390414406364</v>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>USDT</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>9/14/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="n">
+        <v>0.01291898853678397</v>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>UNI</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>9/15/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="n">
+        <v>0.00363001563677328</v>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>WETH</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>9/16/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="n">
+        <v>21.87140912622817</v>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>USDC</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>9/17/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="n">
+        <v>19.20040328892501</v>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>WBTC</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>9/18/2021</t>
         </is>
       </c>
     </row>

</xml_diff>